<commit_message>
fix water faclility xlsx
</commit_message>
<xml_diff>
--- a/data/water_supply_facility/data.xlsx
+++ b/data/water_supply_facility/data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ivpf201v.takamatsu.local\Profile\s11606\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naoppy/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF53A1C-DF26-5C43-8045-60C6E845D2FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24360" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -162,8 +163,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -175,6 +176,14 @@
       <sz val="6"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
@@ -199,9 +208,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -540,19 +550,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="9" max="9" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -590,7 +600,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>1</v>
       </c>
@@ -628,7 +638,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>2</v>
       </c>
@@ -663,7 +673,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>3</v>
       </c>
@@ -691,14 +701,14 @@
       <c r="J4" s="1">
         <v>0.375</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="2">
         <v>0.70833333333333337</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>4</v>
       </c>
@@ -726,14 +736,14 @@
       <c r="J5" s="1">
         <v>0.375</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="2">
         <v>0.70833333333333337</v>
       </c>
       <c r="L5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>5</v>
       </c>
@@ -753,7 +763,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>6</v>
       </c>
@@ -773,7 +783,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>7</v>
       </c>
@@ -796,7 +806,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>8</v>
       </c>
@@ -819,7 +829,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>9</v>
       </c>
@@ -847,7 +857,7 @@
       <c r="J10" s="1">
         <v>0.375</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="2">
         <v>0.70833333333333337</v>
       </c>
       <c r="L10" t="s">
@@ -859,7 +869,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:L1 A6:L9 A2:I2 L2 A3:I3 L3 A4:I4 L4 A5:I5 L5 A10:I10 L10" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:L1 A6:I9 A2:I2 L2 A3:I3 L3 A4:I4 L4 A5:I5 L5 A10:I10 L10 L6:L9" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>